<commit_message>
Small change to PID model file.
</commit_message>
<xml_diff>
--- a/DataAnalysis/PID Model for StoveRegulator.xlsx
+++ b/DataAnalysis/PID Model for StoveRegulator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbuhi\Desktop\arduino\Wood Stove Regulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbuhi\Desktop\GitHub\WoodStoveRegulator\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329695C1-BC47-4D36-B0E9-E70A9CD11056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4B22AA-B9E0-422A-A1FD-23524A36455D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F8C13CFD-1D5C-4526-ACBA-B9B948E6AA87}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -433,7 +435,7 @@
   <dimension ref="A2:AN20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +943,7 @@
         <v>50</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E7">
         <v>80</v>
@@ -1545,7 +1547,7 @@
       </c>
       <c r="D13">
         <f t="shared" ref="D13:AN13" si="14">(D6-D7)</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E13">
         <f t="shared" si="14"/>
@@ -1705,151 +1707,151 @@
       </c>
       <c r="D14">
         <f t="shared" ref="D14:AN14" si="15">(C14+D13)</f>
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E14">
         <f t="shared" si="15"/>
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F14">
         <f t="shared" si="15"/>
+        <v>220</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="15"/>
         <v>230</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="15"/>
-        <v>240</v>
-      </c>
       <c r="H14">
         <f t="shared" si="15"/>
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="I14">
         <f t="shared" si="15"/>
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="J14">
         <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="15"/>
+        <v>222</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="15"/>
         <v>232</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="15"/>
-        <v>232</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="15"/>
-        <v>242</v>
-      </c>
       <c r="X14">
         <f t="shared" si="15"/>
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="Y14">
         <f t="shared" si="15"/>
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="Z14">
         <f t="shared" si="15"/>
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="AA14">
         <f t="shared" si="15"/>
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="AB14">
         <f t="shared" si="15"/>
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="AC14">
         <f t="shared" si="15"/>
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="AD14">
         <f t="shared" si="15"/>
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="AE14">
         <f t="shared" si="15"/>
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="AF14">
         <f t="shared" si="15"/>
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="AG14">
         <f t="shared" si="15"/>
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="AH14">
         <f t="shared" si="15"/>
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="AI14">
         <f t="shared" si="15"/>
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="15"/>
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="AK14">
         <f t="shared" si="15"/>
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="AL14">
         <f t="shared" si="15"/>
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="AM14">
         <f t="shared" si="15"/>
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="AN14">
         <f t="shared" si="15"/>
-        <v>742</v>
+        <v>732</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -2185,11 +2187,11 @@
       </c>
       <c r="D18">
         <f t="shared" ref="D18:AN18" si="22">(D13-D19)</f>
+        <v>-20</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="22"/>
         <v>-10</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="22"/>
-        <v>-20</v>
       </c>
       <c r="F18">
         <f t="shared" si="22"/>
@@ -2349,7 +2351,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="23"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F19">
         <f t="shared" si="23"/>
@@ -2506,151 +2508,151 @@
       </c>
       <c r="D20">
         <f t="shared" si="26"/>
-        <v>350.0745</v>
+        <v>300.06900000000002</v>
       </c>
       <c r="E20">
         <f t="shared" si="26"/>
-        <v>250.09899999999999</v>
+        <v>250.09450000000001</v>
       </c>
       <c r="F20">
         <f>F10*F13+F11*F14+F12*F18</f>
-        <v>150.114</v>
+        <v>150.10900000000001</v>
       </c>
       <c r="G20">
         <f t="shared" si="26"/>
-        <v>50.119</v>
+        <v>50.114000000000004</v>
       </c>
       <c r="H20">
         <f t="shared" si="26"/>
-        <v>-49.885999999999996</v>
+        <v>-49.890999999999998</v>
       </c>
       <c r="I20">
         <f t="shared" ref="I20:T20" si="27">I10*I13+I11*I14+I12*I18</f>
-        <v>25.11825</v>
+        <v>25.113250000000001</v>
       </c>
       <c r="J20">
         <f t="shared" si="27"/>
-        <v>-14.884400000000001</v>
+        <v>-14.8894</v>
       </c>
       <c r="K20">
         <f t="shared" si="27"/>
-        <v>0.11615</v>
+        <v>0.11115</v>
       </c>
       <c r="L20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="M20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="N20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="O20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="P20">
         <f>P10*P13+P11*P14+P12*P18</f>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="Q20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="R20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="S20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="T20">
         <f t="shared" si="27"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="U20">
         <f t="shared" ref="U20:AN20" si="28">U10*U13+U11*U14+U12*U18</f>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="V20">
         <f t="shared" si="28"/>
-        <v>0.11600000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="W20">
         <f t="shared" si="28"/>
-        <v>50.121500000000005</v>
+        <v>50.116500000000002</v>
       </c>
       <c r="X20">
         <f t="shared" si="28"/>
-        <v>100.1315</v>
+        <v>100.12650000000001</v>
       </c>
       <c r="Y20">
         <f t="shared" si="28"/>
-        <v>150.14649999999997</v>
+        <v>150.14149999999998</v>
       </c>
       <c r="Z20">
         <f t="shared" si="28"/>
-        <v>150.161</v>
+        <v>150.15600000000001</v>
       </c>
       <c r="AA20">
         <f t="shared" si="28"/>
-        <v>150.17599999999999</v>
+        <v>150.17099999999999</v>
       </c>
       <c r="AB20">
         <f t="shared" si="28"/>
-        <v>150.191</v>
+        <v>150.18600000000001</v>
       </c>
       <c r="AC20">
         <f t="shared" si="28"/>
-        <v>150.20599999999999</v>
+        <v>150.20099999999999</v>
       </c>
       <c r="AD20">
         <f t="shared" si="28"/>
-        <v>150.221</v>
+        <v>150.21600000000001</v>
       </c>
       <c r="AE20">
         <f t="shared" si="28"/>
-        <v>150.23599999999999</v>
+        <v>150.23099999999999</v>
       </c>
       <c r="AF20">
         <f t="shared" si="28"/>
-        <v>150.251</v>
+        <v>150.24600000000001</v>
       </c>
       <c r="AG20">
         <f t="shared" si="28"/>
-        <v>150.26599999999999</v>
+        <v>150.261</v>
       </c>
       <c r="AH20">
         <f t="shared" si="28"/>
-        <v>150.28100000000001</v>
+        <v>150.27600000000001</v>
       </c>
       <c r="AI20">
         <f t="shared" si="28"/>
-        <v>150.29599999999999</v>
+        <v>150.291</v>
       </c>
       <c r="AJ20">
         <f t="shared" si="28"/>
-        <v>150.31100000000001</v>
+        <v>150.30600000000001</v>
       </c>
       <c r="AK20">
         <f t="shared" si="28"/>
-        <v>150.32599999999999</v>
+        <v>150.321</v>
       </c>
       <c r="AL20">
         <f t="shared" si="28"/>
-        <v>150.34100000000001</v>
+        <v>150.33600000000001</v>
       </c>
       <c r="AM20">
         <f t="shared" si="28"/>
-        <v>150.35599999999999</v>
+        <v>150.351</v>
       </c>
       <c r="AN20">
         <f t="shared" si="28"/>
-        <v>150.37100000000001</v>
+        <v>150.36600000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>